<commit_message>
added work from 17.10.2023
</commit_message>
<xml_diff>
--- a/Year 1 - 2023-2024/Modul 1/Excel/17.10.2023/oborot.xlsx
+++ b/Year 1 - 2023-2024/Modul 1/Excel/17.10.2023/oborot.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DOM\tmp\ivan\informatika\uchebnik_11class\задачи\urok 12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\IT\Year 1 - 2023-2024\Modul 1\Excel\17.10.2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46676F2-E18F-486E-BE5A-CCED385E9FE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A642E1-EC22-4D85-8EFC-3F38550B08F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12075" yWindow="90" windowWidth="13275" windowHeight="15255" xr2:uid="{3AD31903-9B73-4E7F-8592-F07B2D613A09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{3AD31903-9B73-4E7F-8592-F07B2D613A09}"/>
   </bookViews>
   <sheets>
-    <sheet name="магазин" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="магазин" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="11" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +27,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
   <si>
     <t>дата</t>
   </si>
@@ -52,6 +61,51 @@
   </si>
   <si>
     <t>София</t>
+  </si>
+  <si>
+    <t>Sum of стойност</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>(All)</t>
+  </si>
+  <si>
+    <t>Работни дни</t>
+  </si>
+  <si>
+    <t>Почивни дни</t>
+  </si>
+  <si>
+    <t>Бургас</t>
   </si>
 </sst>
 </file>
@@ -59,7 +113,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;лв.&quot;_-;\-* #,##0.00\ &quot;лв.&quot;_-;_-* &quot;-&quot;??\ &quot;лв.&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;лв.&quot;_-;\-* #,##0.00\ &quot;лв.&quot;_-;_-* &quot;-&quot;??\ &quot;лв.&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -120,21 +174,29 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Валута" xfId="1" builtinId="4"/>
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -217,7 +279,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="27" formatCode="d/m/yyyy\ h:mm"/>
+      <numFmt numFmtId="165" formatCode="d/m/yyyy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -247,7 +309,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -294,6 +356,383 @@
 </styleSheet>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Lenovo" refreshedDate="45216.425352430553" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="30" xr:uid="{BF67EB8F-B8B5-42B3-934C-FE8BC162E8FD}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="дата" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2019-10-01T00:00:00" maxDate="2019-10-11T00:00:00" count="10">
+        <d v="2019-10-01T00:00:00"/>
+        <d v="2019-10-02T00:00:00"/>
+        <d v="2019-10-03T00:00:00"/>
+        <d v="2019-10-04T00:00:00"/>
+        <d v="2019-10-05T00:00:00"/>
+        <d v="2019-10-06T00:00:00"/>
+        <d v="2019-10-07T00:00:00"/>
+        <d v="2019-10-08T00:00:00"/>
+        <d v="2019-10-09T00:00:00"/>
+        <d v="2019-10-10T00:00:00"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="ден" numFmtId="22">
+      <sharedItems count="7">
+        <s v="Tuesday"/>
+        <s v="Wednesday"/>
+        <s v="Thursday"/>
+        <s v="Friday"/>
+        <s v="Saturday"/>
+        <s v="Sunday"/>
+        <s v="Monday"/>
+      </sharedItems>
+      <fieldGroup par="4"/>
+    </cacheField>
+    <cacheField name="магазин" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Варна"/>
+        <s v="София"/>
+        <s v="Бургас"/>
+        <s v="Пловдив"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="стойност" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="5648.23" maxValue="20154"/>
+    </cacheField>
+    <cacheField name="ден2" numFmtId="0" databaseField="0">
+      <fieldGroup base="1">
+        <discretePr count="7">
+          <x v="0"/>
+          <x v="0"/>
+          <x v="0"/>
+          <x v="0"/>
+          <x v="1"/>
+          <x v="1"/>
+          <x v="0"/>
+        </discretePr>
+        <groupItems count="2">
+          <s v="Group1"/>
+          <s v="Group2"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="30">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5648.23"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="9785.23"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="7856"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="8965"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="12563"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="11452"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="9685"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="18562"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="12365"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="11452"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="15462"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="12564"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="9685"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="12563"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="10563"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="14569"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="18562"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="16352"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="0"/>
+    <n v="11256"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="19635"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="3"/>
+    <n v="15465"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6985"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="9685"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="8965"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="14526"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="20154"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="14569"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="9685"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="17856"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="15269"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B99E6841-276F-40C9-88F9-1247477E7DAA}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:F14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisPage" numFmtId="14" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="6"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item n="Работни дни" x="0"/>
+        <item n="Почивни дни" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="4"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of стойност" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0B92AD21-E7E5-421C-8209-DB202F09F8FD}" name="Table1" displayName="Table1" ref="A3:D33" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A3:D33" xr:uid="{FECF2979-488C-45F3-9AB5-1688B972A1AA}"/>
@@ -310,9 +749,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема на Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Оffice">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -350,7 +789,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Оffice">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -456,7 +895,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Оffice">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -605,11 +1044,260 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6120E94-AD6B-439A-B89C-82DD08303304}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="6">
+        <v>78202.23</v>
+      </c>
+      <c r="C5" s="6">
+        <v>90649</v>
+      </c>
+      <c r="D5" s="6">
+        <v>105140.23</v>
+      </c>
+      <c r="E5" s="6">
+        <v>26418</v>
+      </c>
+      <c r="F5" s="6">
+        <v>300409.45999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6">
+        <v>11256</v>
+      </c>
+      <c r="C6" s="6">
+        <v>15465</v>
+      </c>
+      <c r="D6" s="6">
+        <v>19635</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6">
+        <v>46356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6">
+        <v>12633.23</v>
+      </c>
+      <c r="C7" s="6">
+        <v>8965</v>
+      </c>
+      <c r="D7" s="6">
+        <v>19470.23</v>
+      </c>
+      <c r="E7" s="6">
+        <v>7856</v>
+      </c>
+      <c r="F7" s="6">
+        <v>48924.46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6">
+        <v>23491</v>
+      </c>
+      <c r="C8" s="6">
+        <v>26021</v>
+      </c>
+      <c r="D8" s="6">
+        <v>32717</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6">
+        <v>82229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6">
+        <v>19370</v>
+      </c>
+      <c r="C9" s="6">
+        <v>27634</v>
+      </c>
+      <c r="D9" s="6">
+        <v>17856</v>
+      </c>
+      <c r="E9" s="6">
+        <v>18562</v>
+      </c>
+      <c r="F9" s="6">
+        <v>83422</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6">
+        <v>11452</v>
+      </c>
+      <c r="C10" s="6">
+        <v>12564</v>
+      </c>
+      <c r="D10" s="6">
+        <v>15462</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6">
+        <v>39478</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6">
+        <v>24254</v>
+      </c>
+      <c r="C11" s="6">
+        <v>16352</v>
+      </c>
+      <c r="D11" s="6">
+        <v>31125</v>
+      </c>
+      <c r="E11" s="6">
+        <v>10563</v>
+      </c>
+      <c r="F11" s="6">
+        <v>82294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="6">
+        <v>9685</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6">
+        <v>12563</v>
+      </c>
+      <c r="E12" s="6">
+        <v>10563</v>
+      </c>
+      <c r="F12" s="6">
+        <v>32811</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="6">
+        <v>14569</v>
+      </c>
+      <c r="C13" s="6">
+        <v>16352</v>
+      </c>
+      <c r="D13" s="6">
+        <v>18562</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6">
+        <v>49483</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="6">
+        <v>102456.23</v>
+      </c>
+      <c r="C14" s="6">
+        <v>107001</v>
+      </c>
+      <c r="D14" s="6">
+        <v>136265.22999999998</v>
+      </c>
+      <c r="E14" s="6">
+        <v>36981</v>
+      </c>
+      <c r="F14" s="6">
+        <v>382703.45999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2D0434-75DD-45C9-BBE8-40B8CF783572}">
   <dimension ref="A3:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,7 +1328,7 @@
       </c>
       <c r="B4" s="4" t="str">
         <f t="shared" ref="B4:B33" si="0">TEXT(A4,"dddd")</f>
-        <v>вторник</v>
+        <v>Tuesday</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -655,7 +1343,7 @@
       </c>
       <c r="B5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>вторник</v>
+        <v>Tuesday</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
@@ -670,10 +1358,10 @@
       </c>
       <c r="B6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>вторник</v>
+        <v>Tuesday</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2">
         <v>7856</v>
@@ -685,7 +1373,7 @@
       </c>
       <c r="B7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>сряда</v>
+        <v>Wednesday</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>4</v>
@@ -700,7 +1388,7 @@
       </c>
       <c r="B8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>сряда</v>
+        <v>Wednesday</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>6</v>
@@ -715,7 +1403,7 @@
       </c>
       <c r="B9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>сряда</v>
+        <v>Wednesday</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>5</v>
@@ -730,7 +1418,7 @@
       </c>
       <c r="B10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>четвъртък</v>
+        <v>Thursday</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>4</v>
@@ -745,10 +1433,10 @@
       </c>
       <c r="B11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>четвъртък</v>
+        <v>Thursday</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D11" s="2">
         <v>18562</v>
@@ -760,7 +1448,7 @@
       </c>
       <c r="B12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>четвъртък</v>
+        <v>Thursday</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>5</v>
@@ -775,7 +1463,7 @@
       </c>
       <c r="B13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>петък</v>
+        <v>Friday</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>4</v>
@@ -790,7 +1478,7 @@
       </c>
       <c r="B14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>петък</v>
+        <v>Friday</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>6</v>
@@ -805,7 +1493,7 @@
       </c>
       <c r="B15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>петък</v>
+        <v>Friday</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>5</v>
@@ -820,7 +1508,7 @@
       </c>
       <c r="B16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>събота</v>
+        <v>Saturday</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>4</v>
@@ -835,7 +1523,7 @@
       </c>
       <c r="B17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>събота</v>
+        <v>Saturday</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>6</v>
@@ -850,10 +1538,10 @@
       </c>
       <c r="B18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>събота</v>
+        <v>Saturday</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D18" s="2">
         <v>10563</v>
@@ -865,7 +1553,7 @@
       </c>
       <c r="B19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>неделя</v>
+        <v>Sunday</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>4</v>
@@ -880,7 +1568,7 @@
       </c>
       <c r="B20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>неделя</v>
+        <v>Sunday</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>6</v>
@@ -895,7 +1583,7 @@
       </c>
       <c r="B21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>неделя</v>
+        <v>Sunday</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>5</v>
@@ -910,7 +1598,7 @@
       </c>
       <c r="B22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>понеделник</v>
+        <v>Monday</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>4</v>
@@ -925,7 +1613,7 @@
       </c>
       <c r="B23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>понеделник</v>
+        <v>Monday</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>6</v>
@@ -940,7 +1628,7 @@
       </c>
       <c r="B24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>понеделник</v>
+        <v>Monday</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>5</v>
@@ -955,7 +1643,7 @@
       </c>
       <c r="B25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>вторник</v>
+        <v>Tuesday</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>4</v>
@@ -970,7 +1658,7 @@
       </c>
       <c r="B26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>вторник</v>
+        <v>Tuesday</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>6</v>
@@ -985,7 +1673,7 @@
       </c>
       <c r="B27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>вторник</v>
+        <v>Tuesday</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>5</v>
@@ -1000,7 +1688,7 @@
       </c>
       <c r="B28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>сряда</v>
+        <v>Wednesday</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>4</v>
@@ -1015,7 +1703,7 @@
       </c>
       <c r="B29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>сряда</v>
+        <v>Wednesday</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>6</v>
@@ -1030,7 +1718,7 @@
       </c>
       <c r="B30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>сряда</v>
+        <v>Wednesday</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>5</v>
@@ -1045,7 +1733,7 @@
       </c>
       <c r="B31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>четвъртък</v>
+        <v>Thursday</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>4</v>
@@ -1060,7 +1748,7 @@
       </c>
       <c r="B32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>четвъртък</v>
+        <v>Thursday</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
@@ -1075,7 +1763,7 @@
       </c>
       <c r="B33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>четвъртък</v>
+        <v>Thursday</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>5</v>

</xml_diff>